<commit_message>
April 14 modifications completed
</commit_message>
<xml_diff>
--- a/funds/1623 Capital/var_data_Firm_20240307.xlsx
+++ b/funds/1623 Capital/var_data_Firm_20240307.xlsx
@@ -2480,7 +2480,7 @@
         <v>21</v>
       </c>
       <c r="F84">
-        <v>0.0008159105299160464</v>
+        <v>0.0008159105299160446</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2540,7 +2540,7 @@
         <v>24</v>
       </c>
       <c r="F87">
-        <v>-5.672213704561134E-05</v>
+        <v>-5.672213704561307E-05</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2980,7 +2980,7 @@
         <v>46</v>
       </c>
       <c r="F109">
-        <v>0.001048822154601645</v>
+        <v>0.001048822154601644</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3100,7 +3100,7 @@
         <v>52</v>
       </c>
       <c r="F115">
-        <v>-0.0001683346579327699</v>
+        <v>-0.0001683346579327682</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3180,7 +3180,7 @@
         <v>56</v>
       </c>
       <c r="F119">
-        <v>0.0003710665805222169</v>
+        <v>0.0003710665805222134</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3200,7 +3200,7 @@
         <v>5</v>
       </c>
       <c r="F120">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -4040,7 +4040,7 @@
         <v>20</v>
       </c>
       <c r="F162">
-        <v>0.0006156534834944823</v>
+        <v>0.0006156534834944822</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -4060,7 +4060,7 @@
         <v>21</v>
       </c>
       <c r="F163">
-        <v>0.0007937445643708903</v>
+        <v>0.0007937445643708902</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -4120,7 +4120,7 @@
         <v>24</v>
       </c>
       <c r="F166">
-        <v>-6.198418413568353E-05</v>
+        <v>-6.198418413568352E-05</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -4160,7 +4160,7 @@
         <v>26</v>
       </c>
       <c r="F168">
-        <v>0.0005968451076066693</v>
+        <v>0.0005968451076066692</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -4180,7 +4180,7 @@
         <v>27</v>
       </c>
       <c r="F169">
-        <v>0.0008481057795720629</v>
+        <v>0.0008481057795720628</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -4200,7 +4200,7 @@
         <v>28</v>
       </c>
       <c r="F170">
-        <v>-0.0006995137780335185</v>
+        <v>-0.0006995137780335184</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -4220,7 +4220,7 @@
         <v>29</v>
       </c>
       <c r="F171">
-        <v>0.0008800983947373233</v>
+        <v>0.0008800983947373232</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -4420,7 +4420,7 @@
         <v>39</v>
       </c>
       <c r="F181">
-        <v>0.0005879323787090721</v>
+        <v>0.000587932378709072</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -4460,7 +4460,7 @@
         <v>41</v>
       </c>
       <c r="F183">
-        <v>0.0006915384457884394</v>
+        <v>0.0006915384457884393</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -4520,7 +4520,7 @@
         <v>44</v>
       </c>
       <c r="F186">
-        <v>-5.419305273187314E-05</v>
+        <v>-5.419305273187313E-05</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -4560,7 +4560,7 @@
         <v>46</v>
       </c>
       <c r="F188">
-        <v>0.0008142581425648913</v>
+        <v>0.0008142581425648912</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -4600,7 +4600,7 @@
         <v>48</v>
       </c>
       <c r="F190">
-        <v>0.0007034621879818265</v>
+        <v>0.0007034621879818264</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -4620,7 +4620,7 @@
         <v>49</v>
       </c>
       <c r="F191">
-        <v>0.0005410532255880043</v>
+        <v>0.0005410532255880042</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -4660,7 +4660,7 @@
         <v>51</v>
       </c>
       <c r="F193">
-        <v>-8.323587603084587E-05</v>
+        <v>-8.323587603084586E-05</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -4700,7 +4700,7 @@
         <v>53</v>
       </c>
       <c r="F195">
-        <v>0.0006037870420990654</v>
+        <v>0.0006037870420990653</v>
       </c>
     </row>
     <row r="196" spans="1:6">
@@ -4720,7 +4720,7 @@
         <v>54</v>
       </c>
       <c r="F196">
-        <v>0.0004739566425456054</v>
+        <v>0.0004739566425456053</v>
       </c>
     </row>
     <row r="197" spans="1:6">
@@ -4780,7 +4780,7 @@
         <v>18</v>
       </c>
       <c r="F199">
-        <v>0.0002099974158281774</v>
+        <v>0.0002099974158281757</v>
       </c>
     </row>
     <row r="200" spans="1:6">
@@ -4800,7 +4800,7 @@
         <v>19</v>
       </c>
       <c r="F200">
-        <v>-0.0003660583320777948</v>
+        <v>-0.0003660583320777965</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -4820,7 +4820,7 @@
         <v>20</v>
       </c>
       <c r="F201">
-        <v>0.000117389598872213</v>
+        <v>0.0001173895988722112</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -4840,7 +4840,7 @@
         <v>21</v>
       </c>
       <c r="F202">
-        <v>0.001153957633594918</v>
+        <v>0.001153957633594915</v>
       </c>
     </row>
     <row r="203" spans="1:6">
@@ -4860,7 +4860,7 @@
         <v>22</v>
       </c>
       <c r="F203">
-        <v>3.425764732322908E-05</v>
+        <v>3.425764732322735E-05</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -4880,7 +4880,7 @@
         <v>23</v>
       </c>
       <c r="F204">
-        <v>-0.0002598495879113719</v>
+        <v>-0.0002598495879113736</v>
       </c>
     </row>
     <row r="205" spans="1:6">
@@ -4900,7 +4900,7 @@
         <v>24</v>
       </c>
       <c r="F205">
-        <v>-8.022318702558678E-05</v>
+        <v>-8.022318702559025E-05</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -4920,7 +4920,7 @@
         <v>25</v>
       </c>
       <c r="F206">
-        <v>-0.001760601973600069</v>
+        <v>-0.001760601973600071</v>
       </c>
     </row>
     <row r="207" spans="1:6">
@@ -4940,7 +4940,7 @@
         <v>26</v>
       </c>
       <c r="F207">
-        <v>0.002280567120780369</v>
+        <v>0.002280567120780367</v>
       </c>
     </row>
     <row r="208" spans="1:6">
@@ -4960,7 +4960,7 @@
         <v>27</v>
       </c>
       <c r="F208">
-        <v>0.001372067064029876</v>
+        <v>0.001372067064029875</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -4980,7 +4980,7 @@
         <v>28</v>
       </c>
       <c r="F209">
-        <v>-0.0007888315852711131</v>
+        <v>-0.0007888315852711148</v>
       </c>
     </row>
     <row r="210" spans="1:6">
@@ -5000,7 +5000,7 @@
         <v>29</v>
       </c>
       <c r="F210">
-        <v>0.0006288376360621614</v>
+        <v>0.0006288376360621597</v>
       </c>
     </row>
     <row r="211" spans="1:6">
@@ -5020,7 +5020,7 @@
         <v>30</v>
       </c>
       <c r="F211">
-        <v>-0.0001200191191616986</v>
+        <v>-0.0001200191191617003</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -5040,7 +5040,7 @@
         <v>31</v>
       </c>
       <c r="F212">
-        <v>-0.0003584217090844069</v>
+        <v>-0.0003584217090844086</v>
       </c>
     </row>
     <row r="213" spans="1:6">
@@ -5060,7 +5060,7 @@
         <v>32</v>
       </c>
       <c r="F213">
-        <v>-0.000272074570938953</v>
+        <v>-0.0002720745709389547</v>
       </c>
     </row>
     <row r="214" spans="1:6">
@@ -5080,7 +5080,7 @@
         <v>33</v>
       </c>
       <c r="F214">
-        <v>0.0001846966048944694</v>
+        <v>0.0001846966048944677</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -5100,7 +5100,7 @@
         <v>34</v>
       </c>
       <c r="F215">
-        <v>0.002128425927293152</v>
+        <v>0.00212842592729315</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -5120,7 +5120,7 @@
         <v>35</v>
       </c>
       <c r="F216">
-        <v>0.0009573406892193926</v>
+        <v>0.0009573406892193909</v>
       </c>
     </row>
     <row r="217" spans="1:6">
@@ -5140,7 +5140,7 @@
         <v>36</v>
       </c>
       <c r="F217">
-        <v>0.0004912276463143253</v>
+        <v>0.0004912276463143236</v>
       </c>
     </row>
     <row r="218" spans="1:6">
@@ -5160,7 +5160,7 @@
         <v>37</v>
       </c>
       <c r="F218">
-        <v>-0.0001131412315838552</v>
+        <v>-0.0001131412315838569</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -5180,7 +5180,7 @@
         <v>38</v>
       </c>
       <c r="F219">
-        <v>-0.000144048671762308</v>
+        <v>-0.0001440486717623098</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -5200,7 +5200,7 @@
         <v>39</v>
       </c>
       <c r="F220">
-        <v>0.0009061756525167389</v>
+        <v>0.0009061756525167372</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -5220,7 +5220,7 @@
         <v>40</v>
       </c>
       <c r="F221">
-        <v>0.001921888164017376</v>
+        <v>0.001921888164017374</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -5240,7 +5240,7 @@
         <v>41</v>
       </c>
       <c r="F222">
-        <v>0.0007526472359021385</v>
+        <v>0.0007526472359021368</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -5260,7 +5260,7 @@
         <v>42</v>
       </c>
       <c r="F223">
-        <v>-0.0002793750588783867</v>
+        <v>-0.0002793750588783884</v>
       </c>
     </row>
     <row r="224" spans="1:6">
@@ -5280,7 +5280,7 @@
         <v>43</v>
       </c>
       <c r="F224">
-        <v>-0.0002016710073401429</v>
+        <v>-0.0002016710073401446</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -5300,7 +5300,7 @@
         <v>44</v>
       </c>
       <c r="F225">
-        <v>-1.355908366307799E-05</v>
+        <v>-1.355908366307973E-05</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -5320,7 +5320,7 @@
         <v>45</v>
       </c>
       <c r="F226">
-        <v>-5.93406794618459E-05</v>
+        <v>-5.934067946184764E-05</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -5340,7 +5340,7 @@
         <v>46</v>
       </c>
       <c r="F227">
-        <v>0.001483368932265861</v>
+        <v>0.001483368932265857</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -5360,7 +5360,7 @@
         <v>47</v>
       </c>
       <c r="F228">
-        <v>-3.563556964144426E-05</v>
+        <v>-3.5635569641446E-05</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -5380,7 +5380,7 @@
         <v>48</v>
       </c>
       <c r="F229">
-        <v>0.0006754349127499858</v>
+        <v>0.000675434912749984</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -5400,7 +5400,7 @@
         <v>49</v>
       </c>
       <c r="F230">
-        <v>0.0003619058388782403</v>
+        <v>0.0003619058388782386</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -5420,7 +5420,7 @@
         <v>50</v>
       </c>
       <c r="F231">
-        <v>1.677339148488562E-05</v>
+        <v>1.677339148488388E-05</v>
       </c>
     </row>
     <row r="232" spans="1:6">
@@ -5440,7 +5440,7 @@
         <v>51</v>
       </c>
       <c r="F232">
-        <v>-9.919537539526679E-05</v>
+        <v>-9.919537539526853E-05</v>
       </c>
     </row>
     <row r="233" spans="1:6">
@@ -5460,7 +5460,7 @@
         <v>52</v>
       </c>
       <c r="F233">
-        <v>-0.0002380788780114093</v>
+        <v>-0.000238078878011411</v>
       </c>
     </row>
     <row r="234" spans="1:6">
@@ -5480,7 +5480,7 @@
         <v>53</v>
       </c>
       <c r="F234">
-        <v>0.0003716514905951762</v>
+        <v>0.0003716514905951745</v>
       </c>
     </row>
     <row r="235" spans="1:6">
@@ -5520,7 +5520,7 @@
         <v>55</v>
       </c>
       <c r="F236">
-        <v>0.0007048028919119202</v>
+        <v>0.0007048028919119185</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -5540,7 +5540,7 @@
         <v>56</v>
       </c>
       <c r="F237">
-        <v>0.0005248064554451027</v>
+        <v>0.0005248064554450975</v>
       </c>
     </row>
     <row r="238" spans="1:6">
@@ -5580,7 +5580,7 @@
         <v>57</v>
       </c>
       <c r="F239">
-        <v>0.0004336016282187091</v>
+        <v>0.000433601628218709</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -7160,7 +7160,7 @@
         <v>58</v>
       </c>
       <c r="F318">
-        <v>0.001048822154601645</v>
+        <v>0.001048822154601644</v>
       </c>
     </row>
     <row r="319" spans="1:6">
@@ -7300,7 +7300,7 @@
         <v>65</v>
       </c>
       <c r="F325">
-        <v>0.0008159105299160464</v>
+        <v>0.0008159105299160446</v>
       </c>
     </row>
     <row r="326" spans="1:6">
@@ -7500,7 +7500,7 @@
         <v>75</v>
       </c>
       <c r="F335">
-        <v>-5.672213704561134E-05</v>
+        <v>-5.672213704561307E-05</v>
       </c>
     </row>
     <row r="336" spans="1:6">
@@ -7520,7 +7520,7 @@
         <v>76</v>
       </c>
       <c r="F336">
-        <v>0.0003710665805222169</v>
+        <v>0.0003710665805222134</v>
       </c>
     </row>
     <row r="337" spans="1:6">
@@ -7660,7 +7660,7 @@
         <v>83</v>
       </c>
       <c r="F343">
-        <v>-0.0001683346579327699</v>
+        <v>-0.0001683346579327682</v>
       </c>
     </row>
     <row r="344" spans="1:6">
@@ -7920,7 +7920,7 @@
         <v>5</v>
       </c>
       <c r="F356">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="357" spans="1:6">
@@ -7940,7 +7940,7 @@
         <v>57</v>
       </c>
       <c r="F357">
-        <v>0.0006132509515150508</v>
+        <v>0.0006132509515150506</v>
       </c>
     </row>
     <row r="358" spans="1:6">
@@ -8740,7 +8740,7 @@
         <v>58</v>
       </c>
       <c r="F397">
-        <v>0.0008142581425648913</v>
+        <v>0.0008142581425648912</v>
       </c>
     </row>
     <row r="398" spans="1:6">
@@ -8760,7 +8760,7 @@
         <v>59</v>
       </c>
       <c r="F398">
-        <v>0.0007034621879818265</v>
+        <v>0.0007034621879818264</v>
       </c>
     </row>
     <row r="399" spans="1:6">
@@ -8780,7 +8780,7 @@
         <v>60</v>
       </c>
       <c r="F399">
-        <v>0.0008481057795720629</v>
+        <v>0.0008481057795720628</v>
       </c>
     </row>
     <row r="400" spans="1:6">
@@ -8880,7 +8880,7 @@
         <v>65</v>
       </c>
       <c r="F404">
-        <v>0.0007937445643708903</v>
+        <v>0.0007937445643708902</v>
       </c>
     </row>
     <row r="405" spans="1:6">
@@ -8900,7 +8900,7 @@
         <v>66</v>
       </c>
       <c r="F405">
-        <v>0.0006915384457884394</v>
+        <v>0.0006915384457884393</v>
       </c>
     </row>
     <row r="406" spans="1:6">
@@ -8920,7 +8920,7 @@
         <v>67</v>
       </c>
       <c r="F406">
-        <v>0.0008800983947373233</v>
+        <v>0.0008800983947373232</v>
       </c>
     </row>
     <row r="407" spans="1:6">
@@ -8940,7 +8940,7 @@
         <v>68</v>
       </c>
       <c r="F407">
-        <v>0.0005410532255880043</v>
+        <v>0.0005410532255880042</v>
       </c>
     </row>
     <row r="408" spans="1:6">
@@ -8960,7 +8960,7 @@
         <v>69</v>
       </c>
       <c r="F408">
-        <v>-8.323587603084587E-05</v>
+        <v>-8.323587603084586E-05</v>
       </c>
     </row>
     <row r="409" spans="1:6">
@@ -9000,7 +9000,7 @@
         <v>71</v>
       </c>
       <c r="F410">
-        <v>0.0006156534834944823</v>
+        <v>0.0006156534834944822</v>
       </c>
     </row>
     <row r="411" spans="1:6">
@@ -9080,7 +9080,7 @@
         <v>75</v>
       </c>
       <c r="F414">
-        <v>-6.198418413568353E-05</v>
+        <v>-6.198418413568352E-05</v>
       </c>
     </row>
     <row r="415" spans="1:6">
@@ -9200,7 +9200,7 @@
         <v>81</v>
       </c>
       <c r="F420">
-        <v>-0.0006995137780335185</v>
+        <v>-0.0006995137780335184</v>
       </c>
     </row>
     <row r="421" spans="1:6">
@@ -9300,7 +9300,7 @@
         <v>86</v>
       </c>
       <c r="F425">
-        <v>0.0005968451076066693</v>
+        <v>0.0005968451076066692</v>
       </c>
     </row>
     <row r="426" spans="1:6">
@@ -9340,7 +9340,7 @@
         <v>88</v>
       </c>
       <c r="F427">
-        <v>0.0004739566425456054</v>
+        <v>0.0004739566425456053</v>
       </c>
     </row>
     <row r="428" spans="1:6">
@@ -9400,7 +9400,7 @@
         <v>91</v>
       </c>
       <c r="F430">
-        <v>-5.419305273187314E-05</v>
+        <v>-5.419305273187313E-05</v>
       </c>
     </row>
     <row r="431" spans="1:6">
@@ -9440,7 +9440,7 @@
         <v>93</v>
       </c>
       <c r="F432">
-        <v>0.0006037870420990654</v>
+        <v>0.0006037870420990653</v>
       </c>
     </row>
     <row r="433" spans="1:6">
@@ -9460,7 +9460,7 @@
         <v>94</v>
       </c>
       <c r="F433">
-        <v>0.0005879323787090721</v>
+        <v>0.000587932378709072</v>
       </c>
     </row>
     <row r="434" spans="1:6">
@@ -9500,7 +9500,7 @@
         <v>57</v>
       </c>
       <c r="F435">
-        <v>-0.000272074570938953</v>
+        <v>-0.0002720745709389547</v>
       </c>
     </row>
     <row r="436" spans="1:6">
@@ -9520,7 +9520,7 @@
         <v>58</v>
       </c>
       <c r="F436">
-        <v>0.001483368932265861</v>
+        <v>0.001483368932265857</v>
       </c>
     </row>
     <row r="437" spans="1:6">
@@ -9540,7 +9540,7 @@
         <v>59</v>
       </c>
       <c r="F437">
-        <v>0.0006754349127499858</v>
+        <v>0.000675434912749984</v>
       </c>
     </row>
     <row r="438" spans="1:6">
@@ -9560,7 +9560,7 @@
         <v>60</v>
       </c>
       <c r="F438">
-        <v>0.001372067064029876</v>
+        <v>0.001372067064029875</v>
       </c>
     </row>
     <row r="439" spans="1:6">
@@ -9580,7 +9580,7 @@
         <v>61</v>
       </c>
       <c r="F439">
-        <v>0.0002099974158281774</v>
+        <v>0.0002099974158281757</v>
       </c>
     </row>
     <row r="440" spans="1:6">
@@ -9600,7 +9600,7 @@
         <v>62</v>
       </c>
       <c r="F440">
-        <v>1.677339148488562E-05</v>
+        <v>1.677339148488388E-05</v>
       </c>
     </row>
     <row r="441" spans="1:6">
@@ -9620,7 +9620,7 @@
         <v>63</v>
       </c>
       <c r="F441">
-        <v>-0.0003584217090844069</v>
+        <v>-0.0003584217090844086</v>
       </c>
     </row>
     <row r="442" spans="1:6">
@@ -9640,7 +9640,7 @@
         <v>64</v>
       </c>
       <c r="F442">
-        <v>0.0007048028919119202</v>
+        <v>0.0007048028919119185</v>
       </c>
     </row>
     <row r="443" spans="1:6">
@@ -9660,7 +9660,7 @@
         <v>65</v>
       </c>
       <c r="F443">
-        <v>0.001153957633594918</v>
+        <v>0.001153957633594915</v>
       </c>
     </row>
     <row r="444" spans="1:6">
@@ -9680,7 +9680,7 @@
         <v>66</v>
       </c>
       <c r="F444">
-        <v>0.0007526472359021385</v>
+        <v>0.0007526472359021368</v>
       </c>
     </row>
     <row r="445" spans="1:6">
@@ -9700,7 +9700,7 @@
         <v>67</v>
       </c>
       <c r="F445">
-        <v>0.0006288376360621614</v>
+        <v>0.0006288376360621597</v>
       </c>
     </row>
     <row r="446" spans="1:6">
@@ -9720,7 +9720,7 @@
         <v>68</v>
       </c>
       <c r="F446">
-        <v>0.0003619058388782403</v>
+        <v>0.0003619058388782386</v>
       </c>
     </row>
     <row r="447" spans="1:6">
@@ -9740,7 +9740,7 @@
         <v>69</v>
       </c>
       <c r="F447">
-        <v>-9.919537539526679E-05</v>
+        <v>-9.919537539526853E-05</v>
       </c>
     </row>
     <row r="448" spans="1:6">
@@ -9760,7 +9760,7 @@
         <v>70</v>
       </c>
       <c r="F448">
-        <v>3.425764732322908E-05</v>
+        <v>3.425764732322735E-05</v>
       </c>
     </row>
     <row r="449" spans="1:6">
@@ -9780,7 +9780,7 @@
         <v>71</v>
       </c>
       <c r="F449">
-        <v>0.000117389598872213</v>
+        <v>0.0001173895988722112</v>
       </c>
     </row>
     <row r="450" spans="1:6">
@@ -9800,7 +9800,7 @@
         <v>72</v>
       </c>
       <c r="F450">
-        <v>-0.000144048671762308</v>
+        <v>-0.0001440486717623098</v>
       </c>
     </row>
     <row r="451" spans="1:6">
@@ -9820,7 +9820,7 @@
         <v>73</v>
       </c>
       <c r="F451">
-        <v>-0.0002598495879113719</v>
+        <v>-0.0002598495879113736</v>
       </c>
     </row>
     <row r="452" spans="1:6">
@@ -9840,7 +9840,7 @@
         <v>74</v>
       </c>
       <c r="F452">
-        <v>0.001921888164017376</v>
+        <v>0.001921888164017374</v>
       </c>
     </row>
     <row r="453" spans="1:6">
@@ -9860,7 +9860,7 @@
         <v>75</v>
       </c>
       <c r="F453">
-        <v>-8.022318702558678E-05</v>
+        <v>-8.022318702559025E-05</v>
       </c>
     </row>
     <row r="454" spans="1:6">
@@ -9880,7 +9880,7 @@
         <v>76</v>
       </c>
       <c r="F454">
-        <v>0.0005248064554451027</v>
+        <v>0.0005248064554450975</v>
       </c>
     </row>
     <row r="455" spans="1:6">
@@ -9900,7 +9900,7 @@
         <v>77</v>
       </c>
       <c r="F455">
-        <v>0.002128425927293152</v>
+        <v>0.00212842592729315</v>
       </c>
     </row>
     <row r="456" spans="1:6">
@@ -9920,7 +9920,7 @@
         <v>78</v>
       </c>
       <c r="F456">
-        <v>-3.563556964144426E-05</v>
+        <v>-3.5635569641446E-05</v>
       </c>
     </row>
     <row r="457" spans="1:6">
@@ -9940,7 +9940,7 @@
         <v>79</v>
       </c>
       <c r="F457">
-        <v>-0.0001200191191616986</v>
+        <v>-0.0001200191191617003</v>
       </c>
     </row>
     <row r="458" spans="1:6">
@@ -9960,7 +9960,7 @@
         <v>80</v>
       </c>
       <c r="F458">
-        <v>-0.001760601973600069</v>
+        <v>-0.001760601973600071</v>
       </c>
     </row>
     <row r="459" spans="1:6">
@@ -9980,7 +9980,7 @@
         <v>81</v>
       </c>
       <c r="F459">
-        <v>-0.0007888315852711131</v>
+        <v>-0.0007888315852711148</v>
       </c>
     </row>
     <row r="460" spans="1:6">
@@ -10000,7 +10000,7 @@
         <v>82</v>
       </c>
       <c r="F460">
-        <v>-0.0001131412315838552</v>
+        <v>-0.0001131412315838569</v>
       </c>
     </row>
     <row r="461" spans="1:6">
@@ -10020,7 +10020,7 @@
         <v>83</v>
       </c>
       <c r="F461">
-        <v>-0.0002380788780114093</v>
+        <v>-0.000238078878011411</v>
       </c>
     </row>
     <row r="462" spans="1:6">
@@ -10040,7 +10040,7 @@
         <v>84</v>
       </c>
       <c r="F462">
-        <v>-0.0002016710073401429</v>
+        <v>-0.0002016710073401446</v>
       </c>
     </row>
     <row r="463" spans="1:6">
@@ -10060,7 +10060,7 @@
         <v>85</v>
       </c>
       <c r="F463">
-        <v>0.0004912276463143253</v>
+        <v>0.0004912276463143236</v>
       </c>
     </row>
     <row r="464" spans="1:6">
@@ -10080,7 +10080,7 @@
         <v>86</v>
       </c>
       <c r="F464">
-        <v>0.002280567120780369</v>
+        <v>0.002280567120780367</v>
       </c>
     </row>
     <row r="465" spans="1:6">
@@ -10100,7 +10100,7 @@
         <v>87</v>
       </c>
       <c r="F465">
-        <v>-5.93406794618459E-05</v>
+        <v>-5.934067946184764E-05</v>
       </c>
     </row>
     <row r="466" spans="1:6">
@@ -10140,7 +10140,7 @@
         <v>89</v>
       </c>
       <c r="F467">
-        <v>-0.0003660583320777948</v>
+        <v>-0.0003660583320777965</v>
       </c>
     </row>
     <row r="468" spans="1:6">
@@ -10160,7 +10160,7 @@
         <v>90</v>
       </c>
       <c r="F468">
-        <v>0.0001846966048944694</v>
+        <v>0.0001846966048944677</v>
       </c>
     </row>
     <row r="469" spans="1:6">
@@ -10180,7 +10180,7 @@
         <v>91</v>
       </c>
       <c r="F469">
-        <v>-1.355908366307799E-05</v>
+        <v>-1.355908366307973E-05</v>
       </c>
     </row>
     <row r="470" spans="1:6">
@@ -10200,7 +10200,7 @@
         <v>92</v>
       </c>
       <c r="F470">
-        <v>-0.0002793750588783867</v>
+        <v>-0.0002793750588783884</v>
       </c>
     </row>
     <row r="471" spans="1:6">
@@ -10220,7 +10220,7 @@
         <v>93</v>
       </c>
       <c r="F471">
-        <v>0.0003716514905951762</v>
+        <v>0.0003716514905951745</v>
       </c>
     </row>
     <row r="472" spans="1:6">
@@ -10240,7 +10240,7 @@
         <v>94</v>
       </c>
       <c r="F472">
-        <v>0.0009061756525167389</v>
+        <v>0.0009061756525167372</v>
       </c>
     </row>
     <row r="473" spans="1:6">
@@ -10260,7 +10260,7 @@
         <v>95</v>
       </c>
       <c r="F473">
-        <v>0.0009573406892193926</v>
+        <v>0.0009573406892193909</v>
       </c>
     </row>
     <row r="474" spans="1:6">
@@ -10360,7 +10360,7 @@
         <v>5</v>
       </c>
       <c r="F478">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="479" spans="1:6">
@@ -10380,7 +10380,7 @@
         <v>96</v>
       </c>
       <c r="F479">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="480" spans="1:6">
@@ -10420,7 +10420,7 @@
         <v>96</v>
       </c>
       <c r="F481">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="482" spans="1:6">
@@ -10840,7 +10840,7 @@
         <v>100</v>
       </c>
       <c r="F502">
-        <v>0.0007871040289211626</v>
+        <v>0.0007871040289211609</v>
       </c>
     </row>
     <row r="503" spans="1:6">
@@ -10940,7 +10940,7 @@
         <v>5</v>
       </c>
       <c r="F507">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="508" spans="1:6">
@@ -11160,7 +11160,7 @@
         <v>99</v>
       </c>
       <c r="F518">
-        <v>0.0007351502724354631</v>
+        <v>0.000735150272435463</v>
       </c>
     </row>
     <row r="519" spans="1:6">
@@ -11220,7 +11220,7 @@
         <v>102</v>
       </c>
       <c r="F521">
-        <v>0.001888360555501196</v>
+        <v>0.001888360555501195</v>
       </c>
     </row>
     <row r="522" spans="1:6">
@@ -11280,7 +11280,7 @@
         <v>97</v>
       </c>
       <c r="F524">
-        <v>-0.002569146343255693</v>
+        <v>-0.002569146343255694</v>
       </c>
     </row>
     <row r="525" spans="1:6">
@@ -11300,7 +11300,7 @@
         <v>98</v>
       </c>
       <c r="F525">
-        <v>0.003386361241666374</v>
+        <v>0.003386361241666372</v>
       </c>
     </row>
     <row r="526" spans="1:6">
@@ -11320,7 +11320,7 @@
         <v>99</v>
       </c>
       <c r="F526">
-        <v>0.0007975341714018657</v>
+        <v>0.000797534171401864</v>
       </c>
     </row>
     <row r="527" spans="1:6">
@@ -11340,7 +11340,7 @@
         <v>100</v>
       </c>
       <c r="F527">
-        <v>0.001113216056545257</v>
+        <v>0.001113216056545253</v>
       </c>
     </row>
     <row r="528" spans="1:6">
@@ -11360,7 +11360,7 @@
         <v>101</v>
       </c>
       <c r="F528">
-        <v>0.002972533846539444</v>
+        <v>0.002972533846539442</v>
       </c>
     </row>
     <row r="529" spans="1:6">
@@ -11380,7 +11380,7 @@
         <v>102</v>
       </c>
       <c r="F529">
-        <v>0.004317279651612872</v>
+        <v>0.00431727965161287</v>
       </c>
     </row>
     <row r="530" spans="1:6">
@@ -11400,7 +11400,7 @@
         <v>103</v>
       </c>
       <c r="F530">
-        <v>0.001985327440183059</v>
+        <v>0.001985327440183057</v>
       </c>
     </row>
     <row r="531" spans="1:6">
@@ -11420,7 +11420,7 @@
         <v>104</v>
       </c>
       <c r="F531">
-        <v>0.0007207327129556962</v>
+        <v>0.0007207327129556945</v>
       </c>
     </row>
     <row r="532" spans="1:6">
@@ -11500,7 +11500,7 @@
         <v>106</v>
       </c>
       <c r="F535">
-        <v>0.0004336016282187091</v>
+        <v>0.000433601628218709</v>
       </c>
     </row>
     <row r="536" spans="1:6">
@@ -12580,7 +12580,7 @@
         <v>105</v>
       </c>
       <c r="F589">
-        <v>0.0008159105299160464</v>
+        <v>0.0008159105299160446</v>
       </c>
     </row>
     <row r="590" spans="1:6">
@@ -12840,7 +12840,7 @@
         <v>117</v>
       </c>
       <c r="F602">
-        <v>-5.672213704561134E-05</v>
+        <v>-5.672213704561307E-05</v>
       </c>
     </row>
     <row r="603" spans="1:6">
@@ -13000,7 +13000,7 @@
         <v>125</v>
       </c>
       <c r="F610">
-        <v>0.0003710665805222169</v>
+        <v>0.0003710665805222134</v>
       </c>
     </row>
     <row r="611" spans="1:6">
@@ -13140,7 +13140,7 @@
         <v>5</v>
       </c>
       <c r="F617">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="618" spans="1:6">
@@ -13200,7 +13200,7 @@
         <v>106</v>
       </c>
       <c r="F620">
-        <v>0.0006132509515150508</v>
+        <v>0.0006132509515150506</v>
       </c>
     </row>
     <row r="621" spans="1:6">
@@ -13720,7 +13720,7 @@
         <v>105</v>
       </c>
       <c r="F646">
-        <v>0.0007937445643708903</v>
+        <v>0.0007937445643708902</v>
       </c>
     </row>
     <row r="647" spans="1:6">
@@ -13800,7 +13800,7 @@
         <v>108</v>
       </c>
       <c r="F650">
-        <v>0.0005968451076066693</v>
+        <v>0.0005968451076066692</v>
       </c>
     </row>
     <row r="651" spans="1:6">
@@ -13820,7 +13820,7 @@
         <v>109</v>
       </c>
       <c r="F651">
-        <v>0.0005410532255880043</v>
+        <v>0.0005410532255880042</v>
       </c>
     </row>
     <row r="652" spans="1:6">
@@ -13840,7 +13840,7 @@
         <v>110</v>
       </c>
       <c r="F652">
-        <v>-5.419305273187314E-05</v>
+        <v>-5.419305273187313E-05</v>
       </c>
     </row>
     <row r="653" spans="1:6">
@@ -13860,7 +13860,7 @@
         <v>111</v>
       </c>
       <c r="F653">
-        <v>0.0006037870420990654</v>
+        <v>0.0006037870420990653</v>
       </c>
     </row>
     <row r="654" spans="1:6">
@@ -13920,7 +13920,7 @@
         <v>114</v>
       </c>
       <c r="F656">
-        <v>0.0004739566425456054</v>
+        <v>0.0004739566425456053</v>
       </c>
     </row>
     <row r="657" spans="1:6">
@@ -13960,7 +13960,7 @@
         <v>116</v>
       </c>
       <c r="F658">
-        <v>0.0002463522302619801</v>
+        <v>0.00024635223026198</v>
       </c>
     </row>
     <row r="659" spans="1:6">
@@ -13980,7 +13980,7 @@
         <v>117</v>
       </c>
       <c r="F659">
-        <v>-6.198418413568353E-05</v>
+        <v>-6.198418413568352E-05</v>
       </c>
     </row>
     <row r="660" spans="1:6">
@@ -14000,7 +14000,7 @@
         <v>118</v>
       </c>
       <c r="F660">
-        <v>0.0006915384457884394</v>
+        <v>0.0006915384457884393</v>
       </c>
     </row>
     <row r="661" spans="1:6">
@@ -14020,7 +14020,7 @@
         <v>119</v>
       </c>
       <c r="F661">
-        <v>0.001388849033398484</v>
+        <v>0.001388849033398483</v>
       </c>
     </row>
     <row r="662" spans="1:6">
@@ -14060,7 +14060,7 @@
         <v>121</v>
       </c>
       <c r="F663">
-        <v>0.0008481057795720629</v>
+        <v>0.0008481057795720628</v>
       </c>
     </row>
     <row r="664" spans="1:6">
@@ -14100,7 +14100,7 @@
         <v>123</v>
       </c>
       <c r="F665">
-        <v>0.0006156534834944823</v>
+        <v>0.0006156534834944822</v>
       </c>
     </row>
     <row r="666" spans="1:6">
@@ -14200,7 +14200,7 @@
         <v>128</v>
       </c>
       <c r="F670">
-        <v>0.0007446114603197198</v>
+        <v>0.0007446114603197197</v>
       </c>
     </row>
     <row r="671" spans="1:6">
@@ -14280,7 +14280,7 @@
         <v>105</v>
       </c>
       <c r="F674">
-        <v>0.001153957633594918</v>
+        <v>0.001153957633594915</v>
       </c>
     </row>
     <row r="675" spans="1:6">
@@ -14300,7 +14300,7 @@
         <v>97</v>
       </c>
       <c r="F675">
-        <v>-0.002569146343255693</v>
+        <v>-0.002569146343255694</v>
       </c>
     </row>
     <row r="676" spans="1:6">
@@ -14320,7 +14320,7 @@
         <v>106</v>
       </c>
       <c r="F676">
-        <v>-0.000272074570938953</v>
+        <v>-0.0002720745709389547</v>
       </c>
     </row>
     <row r="677" spans="1:6">
@@ -14340,7 +14340,7 @@
         <v>107</v>
       </c>
       <c r="F677">
-        <v>3.425764732322908E-05</v>
+        <v>3.425764732322735E-05</v>
       </c>
     </row>
     <row r="678" spans="1:6">
@@ -14360,7 +14360,7 @@
         <v>108</v>
       </c>
       <c r="F678">
-        <v>0.002280567120780369</v>
+        <v>0.002280567120780367</v>
       </c>
     </row>
     <row r="679" spans="1:6">
@@ -14380,7 +14380,7 @@
         <v>109</v>
       </c>
       <c r="F679">
-        <v>0.0003619058388782403</v>
+        <v>0.0003619058388782386</v>
       </c>
     </row>
     <row r="680" spans="1:6">
@@ -14400,7 +14400,7 @@
         <v>110</v>
       </c>
       <c r="F680">
-        <v>-1.355908366307799E-05</v>
+        <v>-1.355908366307973E-05</v>
       </c>
     </row>
     <row r="681" spans="1:6">
@@ -14420,7 +14420,7 @@
         <v>111</v>
       </c>
       <c r="F681">
-        <v>0.0003716514905951762</v>
+        <v>0.0003716514905951745</v>
       </c>
     </row>
     <row r="682" spans="1:6">
@@ -14440,7 +14440,7 @@
         <v>112</v>
       </c>
       <c r="F682">
-        <v>0.0002099974158281774</v>
+        <v>0.0002099974158281757</v>
       </c>
     </row>
     <row r="683" spans="1:6">
@@ -14460,7 +14460,7 @@
         <v>113</v>
       </c>
       <c r="F683">
-        <v>0.0004912276463143253</v>
+        <v>0.0004912276463143236</v>
       </c>
     </row>
     <row r="684" spans="1:6">
@@ -14500,7 +14500,7 @@
         <v>115</v>
       </c>
       <c r="F685">
-        <v>-3.563556964144426E-05</v>
+        <v>-3.5635569641446E-05</v>
       </c>
     </row>
     <row r="686" spans="1:6">
@@ -14520,7 +14520,7 @@
         <v>116</v>
       </c>
       <c r="F686">
-        <v>-0.0001170618367739885</v>
+        <v>-0.0001170618367739903</v>
       </c>
     </row>
     <row r="687" spans="1:6">
@@ -14540,7 +14540,7 @@
         <v>117</v>
       </c>
       <c r="F687">
-        <v>-8.022318702558678E-05</v>
+        <v>-8.022318702559025E-05</v>
       </c>
     </row>
     <row r="688" spans="1:6">
@@ -14560,7 +14560,7 @@
         <v>118</v>
       </c>
       <c r="F688">
-        <v>0.0007526472359021385</v>
+        <v>0.0007526472359021368</v>
       </c>
     </row>
     <row r="689" spans="1:6">
@@ -14580,7 +14580,7 @@
         <v>119</v>
       </c>
       <c r="F689">
-        <v>0.0006210383085687339</v>
+        <v>0.0006210383085687322</v>
       </c>
     </row>
     <row r="690" spans="1:6">
@@ -14600,7 +14600,7 @@
         <v>120</v>
       </c>
       <c r="F690">
-        <v>0.002526650721733163</v>
+        <v>0.002526650721733161</v>
       </c>
     </row>
     <row r="691" spans="1:6">
@@ -14620,7 +14620,7 @@
         <v>121</v>
       </c>
       <c r="F691">
-        <v>0.001372067064029876</v>
+        <v>0.001372067064029875</v>
       </c>
     </row>
     <row r="692" spans="1:6">
@@ -14640,7 +14640,7 @@
         <v>122</v>
       </c>
       <c r="F692">
-        <v>0.003052716868871418</v>
+        <v>0.003052716868871416</v>
       </c>
     </row>
     <row r="693" spans="1:6">
@@ -14660,7 +14660,7 @@
         <v>123</v>
       </c>
       <c r="F693">
-        <v>0.000117389598872213</v>
+        <v>0.0001173895988722112</v>
       </c>
     </row>
     <row r="694" spans="1:6">
@@ -14680,7 +14680,7 @@
         <v>124</v>
       </c>
       <c r="F694">
-        <v>-0.0002598495879113719</v>
+        <v>-0.0002598495879113736</v>
       </c>
     </row>
     <row r="695" spans="1:6">
@@ -14700,7 +14700,7 @@
         <v>125</v>
       </c>
       <c r="F695">
-        <v>0.0005248064554451027</v>
+        <v>0.0005248064554450975</v>
       </c>
     </row>
     <row r="696" spans="1:6">
@@ -14720,7 +14720,7 @@
         <v>126</v>
       </c>
       <c r="F696">
-        <v>-0.0003584217090844069</v>
+        <v>-0.0003584217090844086</v>
       </c>
     </row>
     <row r="697" spans="1:6">
@@ -14740,7 +14740,7 @@
         <v>127</v>
       </c>
       <c r="F697">
-        <v>-0.0001200191191616986</v>
+        <v>-0.0001200191191617003</v>
       </c>
     </row>
     <row r="698" spans="1:6">
@@ -14760,7 +14760,7 @@
         <v>128</v>
       </c>
       <c r="F698">
-        <v>0.001356380516099012</v>
+        <v>0.00135638051609901</v>
       </c>
     </row>
     <row r="699" spans="1:6">
@@ -14780,7 +14780,7 @@
         <v>129</v>
       </c>
       <c r="F699">
-        <v>-0.000144048671762308</v>
+        <v>-0.0001440486717623098</v>
       </c>
     </row>
     <row r="700" spans="1:6">
@@ -14800,7 +14800,7 @@
         <v>130</v>
       </c>
       <c r="F700">
-        <v>-0.0002016710073401429</v>
+        <v>-0.0002016710073401446</v>
       </c>
     </row>
     <row r="701" spans="1:6">
@@ -14820,7 +14820,7 @@
         <v>131</v>
       </c>
       <c r="F701">
-        <v>0.0009573406892193926</v>
+        <v>0.0009573406892193909</v>
       </c>
     </row>
     <row r="702" spans="1:6">
@@ -15280,7 +15280,7 @@
         <v>5</v>
       </c>
       <c r="F724">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="725" spans="1:6">
@@ -15520,7 +15520,7 @@
         <v>136</v>
       </c>
       <c r="F736">
-        <v>0.0006037870420990654</v>
+        <v>0.0006037870420990653</v>
       </c>
     </row>
     <row r="737" spans="1:6">
@@ -15540,7 +15540,7 @@
         <v>137</v>
       </c>
       <c r="F737">
-        <v>0.0005410532255880043</v>
+        <v>0.0005410532255880042</v>
       </c>
     </row>
     <row r="738" spans="1:6">
@@ -15580,7 +15580,7 @@
         <v>132</v>
       </c>
       <c r="F739">
-        <v>0.002316311791548674</v>
+        <v>0.002316311791548672</v>
       </c>
     </row>
     <row r="740" spans="1:6">
@@ -15600,7 +15600,7 @@
         <v>133</v>
       </c>
       <c r="F740">
-        <v>-0.0002610815143072216</v>
+        <v>-0.0002610815143072234</v>
       </c>
     </row>
     <row r="741" spans="1:6">
@@ -15620,7 +15620,7 @@
         <v>134</v>
       </c>
       <c r="F741">
-        <v>-0.0003660583320777948</v>
+        <v>-0.0003660583320777965</v>
       </c>
     </row>
     <row r="742" spans="1:6">
@@ -15640,7 +15640,7 @@
         <v>135</v>
       </c>
       <c r="F742">
-        <v>0.002128425927293152</v>
+        <v>0.00212842592729315</v>
       </c>
     </row>
     <row r="743" spans="1:6">
@@ -15660,7 +15660,7 @@
         <v>136</v>
       </c>
       <c r="F743">
-        <v>0.0003716514905951762</v>
+        <v>0.0003716514905951745</v>
       </c>
     </row>
     <row r="744" spans="1:6">
@@ -15680,7 +15680,7 @@
         <v>137</v>
       </c>
       <c r="F744">
-        <v>0.0003619058388782403</v>
+        <v>0.0003619058388782386</v>
       </c>
     </row>
     <row r="745" spans="1:6">
@@ -15700,7 +15700,7 @@
         <v>138</v>
       </c>
       <c r="F745">
-        <v>0.008607743335674298</v>
+        <v>0.008607743335674295</v>
       </c>
     </row>
     <row r="746" spans="1:6">
@@ -15780,7 +15780,7 @@
         <v>141</v>
       </c>
       <c r="F749">
-        <v>0.0005707441345687803</v>
+        <v>0.0005707441345687801</v>
       </c>
     </row>
     <row r="750" spans="1:6">
@@ -15980,7 +15980,7 @@
         <v>5</v>
       </c>
       <c r="F759">
-        <v>0.01547415574097696</v>
+        <v>0.01547415574097695</v>
       </c>
     </row>
     <row r="760" spans="1:6">
@@ -16040,7 +16040,7 @@
         <v>141</v>
       </c>
       <c r="F762">
-        <v>0.0008072141819066086</v>
+        <v>0.0008072141819066085</v>
       </c>
     </row>
     <row r="763" spans="1:6">
@@ -16080,7 +16080,7 @@
         <v>139</v>
       </c>
       <c r="F764">
-        <v>0.007282966171108523</v>
+        <v>0.007282966171108522</v>
       </c>
     </row>
     <row r="765" spans="1:6">
@@ -16120,7 +16120,7 @@
         <v>141</v>
       </c>
       <c r="F766">
-        <v>-0.0003590786480976162</v>
+        <v>-0.0003590786480976161</v>
       </c>
     </row>
     <row r="767" spans="1:6">
@@ -16160,7 +16160,7 @@
         <v>139</v>
       </c>
       <c r="F768">
-        <v>0.008233308557306303</v>
+        <v>0.0082333085573063</v>
       </c>
     </row>
     <row r="769" spans="1:6">
@@ -16180,7 +16180,7 @@
         <v>140</v>
       </c>
       <c r="F769">
-        <v>0.002443565688781098</v>
+        <v>0.002443565688781096</v>
       </c>
     </row>
     <row r="770" spans="1:6">
@@ -16200,7 +16200,7 @@
         <v>141</v>
       </c>
       <c r="F770">
-        <v>-0.0004194739597936196</v>
+        <v>-0.0004194739597936214</v>
       </c>
     </row>
     <row r="771" spans="1:6">
@@ -16220,7 +16220,7 @@
         <v>142</v>
       </c>
       <c r="F771">
-        <v>0.001399779869263635</v>
+        <v>0.001399779869263634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>